<commit_message>
fix compute date for report in 1c_Buh
</commit_message>
<xml_diff>
--- a/Data/Output/1c8BuhBuf.xlsx
+++ b/Data/Output/1c8BuhBuf.xlsx
@@ -37,13 +37,13 @@
     <x:t>strContractNum</x:t>
   </x:si>
   <x:si>
-    <x:t>9008613428</x:t>
+    <x:t>9017209964</x:t>
   </x:si>
   <x:si>
     <x:t>strSumma</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">637,95 </x:t>
+    <x:t xml:space="preserve">626,86 </x:t>
   </x:si>
   <x:si>
     <x:r>

</xml_diff>

<commit_message>
Fix click's in forms
</commit_message>
<xml_diff>
--- a/Data/Output/1c8BuhBuf.xlsx
+++ b/Data/Output/1c8BuhBuf.xlsx
@@ -37,13 +37,13 @@
     <x:t>strContractNum</x:t>
   </x:si>
   <x:si>
-    <x:t>9017209964</x:t>
+    <x:t>9019579792</x:t>
   </x:si>
   <x:si>
     <x:t>strSumma</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">626,86 </x:t>
+    <x:t xml:space="preserve">634,10 </x:t>
   </x:si>
   <x:si>
     <x:r>

</xml_diff>